<commit_message>
update A1 to SA on figure
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xjh\CodeSpace\paper\FirstPaper\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\root\Codespace\latex\FirstPaper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B315003C-41B3-479F-B268-DB4322CD963A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1A244F-220D-48F8-9BEA-866BA1733C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{860F6B3E-3C53-4C55-9E10-7DE2A6733AD1}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="24" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -96,19 +96,10 @@
     <t>Artix-7</t>
   </si>
   <si>
-    <t>A1</t>
-  </si>
-  <si>
     <t>Spartan-7</t>
   </si>
   <si>
     <t>Kintex-7</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>A3</t>
   </si>
   <si>
     <t>Row Labels</t>
@@ -133,6 +124,15 @@
   </si>
   <si>
     <t>Sum of E/bit(nJ/bit)</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>UA</t>
+  </si>
+  <si>
+    <t>IA</t>
   </si>
 </sst>
 </file>
@@ -287,8 +287,49 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -484,7 +525,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A1</c:v>
+                  <c:v>SA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -606,7 +647,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A2</c:v>
+                  <c:v>UA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -728,7 +769,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A3</c:v>
+                  <c:v>IA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1301,6 +1342,174 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -1317,7 +1526,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A1</c:v>
+                  <c:v>SA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1439,7 +1648,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A2</c:v>
+                  <c:v>UA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1561,7 +1770,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A3</c:v>
+                  <c:v>IA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1979,19 +2188,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2047,19 +2244,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2115,19 +2300,175 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2187,7 +2528,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A1</c:v>
+                  <c:v>SA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2309,7 +2650,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A2</c:v>
+                  <c:v>UA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2431,7 +2772,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A3</c:v>
+                  <c:v>IA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2854,19 +3195,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2922,19 +3251,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2990,19 +3307,175 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -3062,7 +3535,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A1</c:v>
+                  <c:v>SA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3184,7 +3657,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A2</c:v>
+                  <c:v>UA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3306,7 +3779,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A3</c:v>
+                  <c:v>IA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3724,19 +4197,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -3792,19 +4253,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -3860,19 +4309,175 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -3932,7 +4537,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A1</c:v>
+                  <c:v>SA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4054,7 +4659,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A2</c:v>
+                  <c:v>UA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4176,7 +4781,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>A3</c:v>
+                  <c:v>IA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7463,7 +8068,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="xjh" refreshedDate="45266.653087847226" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="9" xr:uid="{2F959C95-6E84-4C9F-9A06-DFD27FC6536F}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="xjh" refreshedDate="45285.839319444443" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="9" xr:uid="{2F959C95-6E84-4C9F-9A06-DFD27FC6536F}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:Q10" sheet="Sheet1"/>
   </cacheSource>
@@ -7476,16 +8081,17 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Design" numFmtId="0">
-      <sharedItems count="3">
-        <s v="A1"/>
-        <s v="A2"/>
-        <s v="A3"/>
+      <sharedItems count="6">
+        <s v="SA"/>
+        <s v="UA"/>
+        <s v="IA"/>
+        <s v="A1" u="1"/>
+        <s v="A2" u="1"/>
+        <s v="A3" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="State(bit)" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="64" maxValue="64" count="1">
-        <n v="64"/>
-      </sharedItems>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="64" maxValue="64"/>
     </cacheField>
     <cacheField name="Key(bit)" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="128" maxValue="128"/>
@@ -7543,7 +8149,7 @@
   <r>
     <x v="0"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="64"/>
     <n v="128"/>
     <n v="144"/>
     <n v="177"/>
@@ -7562,7 +8168,7 @@
   <r>
     <x v="1"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="64"/>
     <n v="128"/>
     <n v="144"/>
     <n v="177"/>
@@ -7581,7 +8187,7 @@
   <r>
     <x v="2"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="64"/>
     <n v="128"/>
     <n v="144"/>
     <n v="178"/>
@@ -7600,7 +8206,7 @@
   <r>
     <x v="1"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="64"/>
     <n v="128"/>
     <n v="157"/>
     <n v="381"/>
@@ -7619,7 +8225,7 @@
   <r>
     <x v="0"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="64"/>
     <n v="128"/>
     <n v="157"/>
     <n v="378"/>
@@ -7638,7 +8244,7 @@
   <r>
     <x v="2"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="64"/>
     <n v="128"/>
     <n v="157"/>
     <n v="377"/>
@@ -7657,7 +8263,7 @@
   <r>
     <x v="2"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="64"/>
     <n v="128"/>
     <n v="201"/>
     <n v="244"/>
@@ -7676,7 +8282,7 @@
   <r>
     <x v="1"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="64"/>
     <n v="128"/>
     <n v="201"/>
     <n v="244"/>
@@ -7695,7 +8301,7 @@
   <r>
     <x v="0"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="64"/>
     <n v="128"/>
     <n v="201"/>
     <n v="243"/>
@@ -7715,7 +8321,205 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{01B54B2C-2537-4BF7-8DD4-1ECA620CC507}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="43">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7B420591-DCF4-4616-91B3-3FB6A70418D4}" name="PivotTable1" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="26">
+  <location ref="I3:M8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="17">
+    <pivotField axis="axisRow" showAll="0" sortType="ascending">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="7">
+        <item m="1" x="3"/>
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of LUT" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="9">
+    <chartFormat chart="18" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="18" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="18" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="20" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="20" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="20" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="20" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="20" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="20" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{01B54B2C-2537-4BF7-8DD4-1ECA620CC507}" name="PivotTable6" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="43">
   <location ref="AF3:AJ8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="17">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -7727,7 +8531,10 @@
       </items>
     </pivotField>
     <pivotField axis="axisCol" showAll="0">
-      <items count="4">
+      <items count="7">
+        <item m="1" x="3"/>
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -7772,13 +8579,13 @@
   </colFields>
   <colItems count="4">
     <i>
-      <x/>
+      <x v="3"/>
     </i>
     <i>
-      <x v="1"/>
+      <x v="4"/>
     </i>
     <i>
-      <x v="2"/>
+      <x v="5"/>
     </i>
     <i t="grand">
       <x/>
@@ -7787,7 +8594,7 @@
   <dataFields count="1">
     <dataField name="Sum of E/bit(nJ/bit)" fld="16" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="3">
+  <chartFormats count="6">
     <chartFormat chart="37" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -7824,6 +8631,42 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="37" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="37" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="37" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -7837,8 +8680,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{24BD12C7-DDED-40ED-86AA-D40CC005CAB8}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="37">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{24BD12C7-DDED-40ED-86AA-D40CC005CAB8}" name="PivotTable5" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="37">
   <location ref="Y3:AC8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="17">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -7850,7 +8693,10 @@
       </items>
     </pivotField>
     <pivotField axis="axisCol" showAll="0">
-      <items count="4">
+      <items count="7">
+        <item m="1" x="3"/>
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -7895,13 +8741,13 @@
   </colFields>
   <colItems count="4">
     <i>
-      <x/>
+      <x v="3"/>
     </i>
     <i>
-      <x v="1"/>
+      <x v="4"/>
     </i>
     <i>
-      <x v="2"/>
+      <x v="5"/>
     </i>
     <i t="grand">
       <x/>
@@ -7910,7 +8756,7 @@
   <dataFields count="1">
     <dataField name="Sum of FMAX(MHz)" fld="8" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="3">
+  <chartFormats count="6">
     <chartFormat chart="33" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -7947,6 +8793,42 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="33" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="33" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="33" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -7960,8 +8842,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FB4B1C3A-7D45-4C95-95DD-3DEF74A544E4}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="33">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FB4B1C3A-7D45-4C95-95DD-3DEF74A544E4}" name="PivotTable3" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="33">
   <location ref="Q3:U8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="17">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -7973,7 +8855,10 @@
       </items>
     </pivotField>
     <pivotField axis="axisCol" showAll="0">
-      <items count="4">
+      <items count="7">
+        <item m="1" x="3"/>
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -8018,13 +8903,13 @@
   </colFields>
   <colItems count="4">
     <i>
-      <x/>
+      <x v="3"/>
     </i>
     <i>
-      <x v="1"/>
+      <x v="4"/>
     </i>
     <i>
-      <x v="2"/>
+      <x v="5"/>
     </i>
     <i t="grand">
       <x/>
@@ -8033,7 +8918,7 @@
   <dataFields count="1">
     <dataField name="Sum of Slices" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="3">
+  <chartFormats count="6">
     <chartFormat chart="25" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -8070,6 +8955,42 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="25" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="25" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="25" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -8083,8 +9004,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CE9A6251-2391-4703-8708-B5952C51AD25}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="23">
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CE9A6251-2391-4703-8708-B5952C51AD25}" name="PivotTable2" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="23">
   <location ref="A3:E8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="17">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -8096,7 +9017,10 @@
       </items>
     </pivotField>
     <pivotField axis="axisCol" showAll="0">
-      <items count="4">
+      <items count="7">
+        <item m="1" x="3"/>
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -8141,13 +9065,13 @@
   </colFields>
   <colItems count="4">
     <i>
-      <x/>
+      <x v="3"/>
     </i>
     <i>
-      <x v="1"/>
+      <x v="4"/>
     </i>
     <i>
-      <x v="2"/>
+      <x v="5"/>
     </i>
     <i t="grand">
       <x/>
@@ -8263,165 +9187,6 @@
       </pivotArea>
     </chartFormat>
     <chartFormat chart="18" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7B420591-DCF4-4616-91B3-3FB6A70418D4}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="26">
-  <location ref="I3:M8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="17">
-    <pivotField axis="axisRow" showAll="0" sortType="ascending">
-      <items count="4">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of LUT" fld="5" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="6">
-    <chartFormat chart="18" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="18" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="18" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="20" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="20" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="20" format="2" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -8746,20 +9511,20 @@
   <dimension ref="A3:AJ8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AG36" sqref="AG36"/>
+      <selection activeCell="AF36" sqref="AF36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5" customWidth="1"/>
-    <col min="11" max="11" width="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="4" bestFit="1" customWidth="1"/>
@@ -8776,142 +9541,142 @@
   <sheetData>
     <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="AG3" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
       <c r="I4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="K4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" t="s">
         <v>21</v>
       </c>
-      <c r="L4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" t="s">
-        <v>24</v>
-      </c>
       <c r="Q4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="S4" t="s">
+        <v>29</v>
+      </c>
+      <c r="T4" t="s">
+        <v>30</v>
+      </c>
+      <c r="U4" t="s">
         <v>21</v>
       </c>
-      <c r="T4" t="s">
-        <v>22</v>
-      </c>
-      <c r="U4" t="s">
-        <v>24</v>
-      </c>
       <c r="Y4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="Z4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="AA4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC4" t="s">
         <v>21</v>
       </c>
-      <c r="AB4" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>24</v>
-      </c>
       <c r="AF4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="AG4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="AH4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ4" t="s">
         <v>21</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>22</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>144</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>157</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>201</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <v>502</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="5">
         <v>177</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="5">
         <v>378</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="5">
         <v>243</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="5">
         <v>798</v>
       </c>
       <c r="Q5" s="4" t="s">
@@ -8962,37 +9727,37 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6">
+        <v>19</v>
+      </c>
+      <c r="B6" s="5">
         <v>144</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>157</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>201</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="5">
         <v>502</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6">
+        <v>19</v>
+      </c>
+      <c r="J6" s="5">
         <v>178</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="5">
         <v>377</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="5">
         <v>244</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="5">
         <v>799</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R6" s="5">
         <v>58</v>
@@ -9007,7 +9772,7 @@
         <v>241</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Z6" s="5">
         <v>853.97</v>
@@ -9022,7 +9787,7 @@
         <v>1387</v>
       </c>
       <c r="AF6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AG6" s="5">
         <v>27.91</v>
@@ -9039,37 +9804,37 @@
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7">
+        <v>18</v>
+      </c>
+      <c r="B7" s="5">
         <v>144</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="5">
         <v>157</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="5">
         <v>201</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="5">
         <v>502</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7">
+        <v>18</v>
+      </c>
+      <c r="J7" s="5">
         <v>177</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="5">
         <v>381</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="5">
         <v>244</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="5">
         <v>802</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R7" s="5">
         <v>57</v>
@@ -9084,7 +9849,7 @@
         <v>245</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Z7" s="5">
         <v>525.76</v>
@@ -9099,7 +9864,7 @@
         <v>960.91000000000008</v>
       </c>
       <c r="AF7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AG7" s="5">
         <v>26.96</v>
@@ -9116,37 +9881,37 @@
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8">
+        <v>21</v>
+      </c>
+      <c r="B8" s="5">
         <v>432</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>471</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>603</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="5">
         <v>1506</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8">
+        <v>21</v>
+      </c>
+      <c r="J8" s="5">
         <v>532</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="5">
         <v>1136</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="5">
         <v>731</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="5">
         <v>2399</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="R8" s="5">
         <v>174</v>
@@ -9161,7 +9926,7 @@
         <v>726</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="Z8" s="5">
         <v>1937.14</v>
@@ -9176,7 +9941,7 @@
         <v>3321.74</v>
       </c>
       <c r="AF8" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="AG8" s="5">
         <v>81.64</v>
@@ -9202,7 +9967,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9265,7 +10030,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1">
         <v>64</v>
@@ -9315,10 +10080,10 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1">
         <v>64</v>
@@ -9368,10 +10133,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1">
         <v>64</v>
@@ -9421,10 +10186,10 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1">
         <v>64</v>
@@ -9477,7 +10242,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1">
         <v>64</v>
@@ -9527,10 +10292,10 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1">
         <v>64</v>
@@ -9580,10 +10345,10 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1">
         <v>64</v>
@@ -9633,10 +10398,10 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1">
         <v>64</v>
@@ -9689,7 +10454,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1">
         <v>64</v>

</xml_diff>